<commit_message>
Update ST_MP for XLS
</commit_message>
<xml_diff>
--- a/braph2genesis/workflows/structural multiplex/example data ST_MP (MRI)/xls/GroupName1/ST_MP1.xlsx
+++ b/braph2genesis/workflows/structural multiplex/example data ST_MP (MRI)/xls/GroupName1/ST_MP1.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="225">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -683,16 +684,29 @@
   </si>
   <si>
     <t xml:space="preserve">Notes 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -714,6 +728,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -758,13 +780,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -786,8 +824,8 @@
   </sheetPr>
   <dimension ref="A1:BS51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BK14" activeCellId="0" sqref="BK14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BK14" activeCellId="1" sqref="A:C BK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11766,4 +11804,593 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:C"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>62.1054773543024</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>75.1855069227158</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>92.5152796289437</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>82.1512236087026</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>80.5648844927303</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>93.1721261588188</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>84.8900440381544</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>77.3477134844947</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>92.6601061700008</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>52.6838730613414</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>62.0920555359257</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>94.4006019791127</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>84.7493029442311</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>71.3909434981007</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>80.6404799999278</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>68.7620639719139</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>67.1067141301931</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>59.5971675083843</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>67.2322095110364</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>51.3350488179546</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>71.2544479287833</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>65.0017709079704</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>93.9130161849495</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>74.994959237889</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>88.0836637002607</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>68.3628572480859</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>70.7908173698251</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>87.1838024380894</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>94.6041439940935</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>73.5776442168623</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>91.6446600334151</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>83.2559837684866</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>75.5343525277364</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>93.5949948324308</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>87.1024738918515</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>93.1824175549047</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>79.085572944981</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>67.0808068448129</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>71.4458606396148</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>91.0350415625323</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>50.6684235095543</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>57.0512231255283</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>71.2205544438431</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>74.4346262680365</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>52.6860964573613</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>79.6113637532637</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>90.0335886520569</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>54.9334672751845</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>69.6997901398151</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>62.6103540323295</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>